<commit_message>
changed totinflow to inflow
</commit_message>
<xml_diff>
--- a/ppLFER_MUM/OPECHEMSUMM.xlsx
+++ b/ppLFER_MUM/OPECHEMSUMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tim Rodgers\Documents\GitHub\ppLFERMUM\ppLFER_MUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0232CCDA-B335-468E-956A-3B89CCAB7438}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D442F4E-2AC0-4EF5-8C65-EC829DC96F01}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,12 +82,6 @@
     <t>WatEmiss</t>
   </si>
   <si>
-    <t>UairTotInflow</t>
-  </si>
-  <si>
-    <t>LairTotInflow</t>
-  </si>
-  <si>
     <t>WatInflow</t>
   </si>
   <si>
@@ -278,6 +272,12 @@
   </si>
   <si>
     <t>C1=C(C(=CC(=C1Cl)Cl)Cl)C2=CC(=C(C(=C2Cl)Cl)Cl)Cl</t>
+  </si>
+  <si>
+    <t>UairInflow</t>
+  </si>
+  <si>
+    <t>LairInflow</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:AL17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,63 +1207,63 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
         <v>362</v>
@@ -1369,15 +1369,15 @@
         <v>1.5</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>398</v>
@@ -1483,15 +1483,15 @@
         <v>1.5</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
         <v>285</v>
@@ -1597,15 +1597,15 @@
         <v>1.5</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
         <v>328</v>
@@ -1711,15 +1711,15 @@
         <v>1.5</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1">
         <v>431</v>
@@ -1825,15 +1825,15 @@
         <v>1.5</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1">
         <v>326</v>
@@ -1939,15 +1939,15 @@
         <v>1.5</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>406.9</v>
@@ -2053,15 +2053,15 @@
       </c>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1">
         <v>485.8</v>
@@ -2167,15 +2167,15 @@
       </c>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AL9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1">
         <v>564.69100000000003</v>
@@ -2281,15 +2281,15 @@
       </c>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AL10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1">
         <v>643.58000000000004</v>
@@ -2395,15 +2395,15 @@
       </c>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1">
         <v>722.48</v>
@@ -2509,15 +2509,15 @@
       </c>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1">
         <v>257.54000000000002</v>
@@ -2623,15 +2623,15 @@
       </c>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AL13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1">
         <v>291.99</v>
@@ -2737,15 +2737,15 @@
       </c>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AL14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1">
         <v>326.43</v>
@@ -2851,15 +2851,15 @@
       </c>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AL15" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1">
         <v>360.9</v>
@@ -2965,15 +2965,15 @@
       </c>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AL16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1">
         <v>395.32</v>
@@ -3079,10 +3079,10 @@
       </c>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AL17" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>